<commit_message>
buoi hop ngay 29/7
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InternAtwoM\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59C12E1-0003-4AD9-B9E6-7AE75EECBED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880299A1-C499-4FEC-AA5B-7B9F81C32804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{78C26181-3197-4AC1-B1A0-F8D659C78093}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Nhóm 2</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Quân: Làm slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erd + class : diagram </t>
   </si>
 </sst>
 </file>
@@ -156,7 +159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -171,6 +174,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -497,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E41A48-58C5-48BC-8F73-F4E51E05CF77}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +531,7 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -538,7 +544,7 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -549,7 +555,7 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -573,24 +579,24 @@
       <c r="G5" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -612,10 +618,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="8">
         <v>45490</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -623,15 +629,15 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
@@ -645,10 +651,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="8">
         <v>45492</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -656,17 +662,25 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="7"/>
       <c r="C18" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>45502</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>